<commit_message>
chore: update xl_db & test cases
</commit_message>
<xml_diff>
--- a/mock/test.xlsx
+++ b/mock/test.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="13140"/>
+    <workbookView windowWidth="27165" windowHeight="13140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="dev" sheetId="2" r:id="rId2"/>
+    <sheet name="data_t" sheetId="3" r:id="rId2"/>
+    <sheet name="dev" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="745">
   <si>
     <t>id</t>
   </si>
@@ -2257,11 +2258,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -2270,22 +2271,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -2299,8 +2286,90 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2316,28 +2385,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2350,76 +2421,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -2427,6 +2428,72 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2442,67 +2509,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2514,37 +2533,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2562,25 +2563,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2592,25 +2605,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2627,19 +2628,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2661,8 +2666,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2707,174 +2714,168 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="49" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="49" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3197,8 +3198,8 @@
   <sheetPr/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" tabSelected="1" zoomScalePageLayoutView="0" zoomScaleSheetLayoutView="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="I1" sqref="I$1:J$1048576"/>
+    <sheetView showOutlineSymbols="0" zoomScalePageLayoutView="0" zoomScaleSheetLayoutView="0" showWhiteSpace="0" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:K101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6433,15 +6434,3060 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:CW11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:101">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1">
+        <v>32</v>
+      </c>
+      <c r="AH1">
+        <v>33</v>
+      </c>
+      <c r="AI1">
+        <v>34</v>
+      </c>
+      <c r="AJ1">
+        <v>35</v>
+      </c>
+      <c r="AK1">
+        <v>36</v>
+      </c>
+      <c r="AL1">
+        <v>37</v>
+      </c>
+      <c r="AM1">
+        <v>38</v>
+      </c>
+      <c r="AN1">
+        <v>39</v>
+      </c>
+      <c r="AO1">
+        <v>40</v>
+      </c>
+      <c r="AP1">
+        <v>41</v>
+      </c>
+      <c r="AQ1">
+        <v>42</v>
+      </c>
+      <c r="AR1">
+        <v>43</v>
+      </c>
+      <c r="AS1">
+        <v>44</v>
+      </c>
+      <c r="AT1">
+        <v>45</v>
+      </c>
+      <c r="AU1">
+        <v>46</v>
+      </c>
+      <c r="AV1">
+        <v>47</v>
+      </c>
+      <c r="AW1">
+        <v>48</v>
+      </c>
+      <c r="AX1">
+        <v>49</v>
+      </c>
+      <c r="AY1">
+        <v>50</v>
+      </c>
+      <c r="AZ1">
+        <v>51</v>
+      </c>
+      <c r="BA1">
+        <v>52</v>
+      </c>
+      <c r="BB1">
+        <v>53</v>
+      </c>
+      <c r="BC1">
+        <v>54</v>
+      </c>
+      <c r="BD1">
+        <v>55</v>
+      </c>
+      <c r="BE1">
+        <v>56</v>
+      </c>
+      <c r="BF1">
+        <v>57</v>
+      </c>
+      <c r="BG1">
+        <v>58</v>
+      </c>
+      <c r="BH1">
+        <v>59</v>
+      </c>
+      <c r="BI1">
+        <v>60</v>
+      </c>
+      <c r="BJ1">
+        <v>61</v>
+      </c>
+      <c r="BK1">
+        <v>62</v>
+      </c>
+      <c r="BL1">
+        <v>63</v>
+      </c>
+      <c r="BM1">
+        <v>64</v>
+      </c>
+      <c r="BN1">
+        <v>65</v>
+      </c>
+      <c r="BO1">
+        <v>66</v>
+      </c>
+      <c r="BP1">
+        <v>67</v>
+      </c>
+      <c r="BQ1">
+        <v>68</v>
+      </c>
+      <c r="BR1">
+        <v>69</v>
+      </c>
+      <c r="BS1">
+        <v>70</v>
+      </c>
+      <c r="BT1">
+        <v>71</v>
+      </c>
+      <c r="BU1">
+        <v>72</v>
+      </c>
+      <c r="BV1">
+        <v>73</v>
+      </c>
+      <c r="BW1">
+        <v>74</v>
+      </c>
+      <c r="BX1">
+        <v>75</v>
+      </c>
+      <c r="BY1">
+        <v>76</v>
+      </c>
+      <c r="BZ1">
+        <v>77</v>
+      </c>
+      <c r="CA1">
+        <v>78</v>
+      </c>
+      <c r="CB1">
+        <v>79</v>
+      </c>
+      <c r="CC1">
+        <v>80</v>
+      </c>
+      <c r="CD1">
+        <v>81</v>
+      </c>
+      <c r="CE1">
+        <v>82</v>
+      </c>
+      <c r="CF1">
+        <v>83</v>
+      </c>
+      <c r="CG1">
+        <v>84</v>
+      </c>
+      <c r="CH1">
+        <v>85</v>
+      </c>
+      <c r="CI1">
+        <v>86</v>
+      </c>
+      <c r="CJ1">
+        <v>87</v>
+      </c>
+      <c r="CK1">
+        <v>88</v>
+      </c>
+      <c r="CL1">
+        <v>89</v>
+      </c>
+      <c r="CM1">
+        <v>90</v>
+      </c>
+      <c r="CN1">
+        <v>91</v>
+      </c>
+      <c r="CO1">
+        <v>92</v>
+      </c>
+      <c r="CP1">
+        <v>93</v>
+      </c>
+      <c r="CQ1">
+        <v>94</v>
+      </c>
+      <c r="CR1">
+        <v>95</v>
+      </c>
+      <c r="CS1">
+        <v>96</v>
+      </c>
+      <c r="CT1">
+        <v>97</v>
+      </c>
+      <c r="CU1">
+        <v>98</v>
+      </c>
+      <c r="CV1">
+        <v>99</v>
+      </c>
+      <c r="CW1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:101">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" t="s">
+        <v>110</v>
+      </c>
+      <c r="P2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>127</v>
+      </c>
+      <c r="R2" t="s">
+        <v>134</v>
+      </c>
+      <c r="S2" t="s">
+        <v>141</v>
+      </c>
+      <c r="T2" t="s">
+        <v>148</v>
+      </c>
+      <c r="U2" t="s">
+        <v>155</v>
+      </c>
+      <c r="V2" t="s">
+        <v>162</v>
+      </c>
+      <c r="W2" t="s">
+        <v>170</v>
+      </c>
+      <c r="X2" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>192</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>208</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>223</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>260</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>268</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>276</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>282</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>290</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>296</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>302</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>309</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>317</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>324</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>331</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>339</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>347</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>355</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>362</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>369</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>390</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>397</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>405</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>412</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>419</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>426</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>434</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>442</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>450</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>457</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>463</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>469</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>477</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>485</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>492</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>498</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>506</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>514</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>529</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>536</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>544</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>552</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>560</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>574</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>582</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>588</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>595</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>602</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>609</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>616</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>623</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>630</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>636</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>642</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>650</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>657</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>664</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>679</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>686</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>694</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>702</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>710</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>718</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>405</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>731</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="3" spans="1:101">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O3" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>128</v>
+      </c>
+      <c r="R3" t="s">
+        <v>135</v>
+      </c>
+      <c r="S3" t="s">
+        <v>142</v>
+      </c>
+      <c r="T3" t="s">
+        <v>149</v>
+      </c>
+      <c r="U3" t="s">
+        <v>156</v>
+      </c>
+      <c r="V3" t="s">
+        <v>163</v>
+      </c>
+      <c r="W3" t="s">
+        <v>171</v>
+      </c>
+      <c r="X3" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>193</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>239</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>246</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>254</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>261</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>269</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>277</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>283</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>291</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>297</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>303</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>310</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>318</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>332</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>340</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>356</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>363</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>370</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>377</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>384</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>391</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>398</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>406</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>413</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>420</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>427</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>435</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>443</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>451</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>458</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>464</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>470</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>478</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>486</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>202</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>499</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>507</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>515</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>398</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>530</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>537</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>545</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>553</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>561</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>567</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>575</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>583</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>589</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>596</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>603</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>610</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>617</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>624</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>631</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>637</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>643</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>651</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>658</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>665</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>672</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>680</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>687</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>695</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>703</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>711</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>719</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>726</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>732</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:101">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M4" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O4" t="s">
+        <v>112</v>
+      </c>
+      <c r="P4" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>129</v>
+      </c>
+      <c r="R4" t="s">
+        <v>136</v>
+      </c>
+      <c r="S4" t="s">
+        <v>143</v>
+      </c>
+      <c r="T4" t="s">
+        <v>150</v>
+      </c>
+      <c r="U4" t="s">
+        <v>157</v>
+      </c>
+      <c r="V4" t="s">
+        <v>164</v>
+      </c>
+      <c r="W4" t="s">
+        <v>172</v>
+      </c>
+      <c r="X4" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>247</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>262</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>278</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>284</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>298</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>304</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>311</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>319</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>326</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>341</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>349</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>357</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>364</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>371</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>378</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>385</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>392</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>399</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>407</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>414</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>421</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>428</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>436</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>444</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>452</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>459</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>465</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>471</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>479</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>487</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>493</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>500</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>508</v>
+      </c>
+      <c r="BR4" t="s">
+        <v>516</v>
+      </c>
+      <c r="BS4" t="s">
+        <v>523</v>
+      </c>
+      <c r="BT4" t="s">
+        <v>531</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>538</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>546</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>554</v>
+      </c>
+      <c r="BX4" t="s">
+        <v>562</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>568</v>
+      </c>
+      <c r="BZ4" t="s">
+        <v>576</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>584</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>590</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>597</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>604</v>
+      </c>
+      <c r="CE4" t="s">
+        <v>611</v>
+      </c>
+      <c r="CF4" t="s">
+        <v>618</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>625</v>
+      </c>
+      <c r="CH4" t="s">
+        <v>632</v>
+      </c>
+      <c r="CI4" t="s">
+        <v>638</v>
+      </c>
+      <c r="CJ4" t="s">
+        <v>644</v>
+      </c>
+      <c r="CK4" t="s">
+        <v>652</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>659</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>666</v>
+      </c>
+      <c r="CN4" t="s">
+        <v>673</v>
+      </c>
+      <c r="CO4" t="s">
+        <v>681</v>
+      </c>
+      <c r="CP4" t="s">
+        <v>688</v>
+      </c>
+      <c r="CQ4" t="s">
+        <v>696</v>
+      </c>
+      <c r="CR4" t="s">
+        <v>704</v>
+      </c>
+      <c r="CS4" t="s">
+        <v>712</v>
+      </c>
+      <c r="CT4" t="s">
+        <v>720</v>
+      </c>
+      <c r="CU4" t="s">
+        <v>727</v>
+      </c>
+      <c r="CV4" t="s">
+        <v>733</v>
+      </c>
+      <c r="CW4" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="5" spans="1:101">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" t="s">
+        <v>113</v>
+      </c>
+      <c r="P5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>113</v>
+      </c>
+      <c r="R5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" t="s">
+        <v>84</v>
+      </c>
+      <c r="T5" t="s">
+        <v>84</v>
+      </c>
+      <c r="U5" t="s">
+        <v>113</v>
+      </c>
+      <c r="V5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5" t="s">
+        <v>75</v>
+      </c>
+      <c r="X5" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>195</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>195</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>46</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>21</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>195</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>37</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>46</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>113</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>195</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>195</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>113</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>14</v>
+      </c>
+      <c r="BU5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BV5" t="s">
+        <v>46</v>
+      </c>
+      <c r="BW5" t="s">
+        <v>14</v>
+      </c>
+      <c r="BX5" t="s">
+        <v>84</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>195</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>84</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>21</v>
+      </c>
+      <c r="CB5" t="s">
+        <v>46</v>
+      </c>
+      <c r="CC5" t="s">
+        <v>46</v>
+      </c>
+      <c r="CD5" t="s">
+        <v>37</v>
+      </c>
+      <c r="CE5" t="s">
+        <v>195</v>
+      </c>
+      <c r="CF5" t="s">
+        <v>14</v>
+      </c>
+      <c r="CG5" t="s">
+        <v>113</v>
+      </c>
+      <c r="CH5" t="s">
+        <v>195</v>
+      </c>
+      <c r="CI5" t="s">
+        <v>46</v>
+      </c>
+      <c r="CJ5" t="s">
+        <v>14</v>
+      </c>
+      <c r="CK5" t="s">
+        <v>84</v>
+      </c>
+      <c r="CL5" t="s">
+        <v>46</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>113</v>
+      </c>
+      <c r="CN5" t="s">
+        <v>113</v>
+      </c>
+      <c r="CO5" t="s">
+        <v>14</v>
+      </c>
+      <c r="CP5" t="s">
+        <v>37</v>
+      </c>
+      <c r="CQ5" t="s">
+        <v>14</v>
+      </c>
+      <c r="CR5" t="s">
+        <v>37</v>
+      </c>
+      <c r="CS5" t="s">
+        <v>46</v>
+      </c>
+      <c r="CT5" t="s">
+        <v>37</v>
+      </c>
+      <c r="CU5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CV5" t="s">
+        <v>21</v>
+      </c>
+      <c r="CW5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:101">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" t="s">
+        <v>99</v>
+      </c>
+      <c r="O6" t="s">
+        <v>114</v>
+      </c>
+      <c r="P6" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6" t="s">
+        <v>137</v>
+      </c>
+      <c r="S6" t="s">
+        <v>144</v>
+      </c>
+      <c r="T6" t="s">
+        <v>151</v>
+      </c>
+      <c r="U6" t="s">
+        <v>158</v>
+      </c>
+      <c r="V6" t="s">
+        <v>165</v>
+      </c>
+      <c r="W6" t="s">
+        <v>173</v>
+      </c>
+      <c r="X6" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>256</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>263</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>285</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>293</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>299</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>305</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>312</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>327</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>334</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>350</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>358</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>365</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>372</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>379</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>386</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>393</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>400</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>408</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>415</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>422</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>429</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>437</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>445</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>453</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>460</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>466</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>472</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>480</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>488</v>
+      </c>
+      <c r="BO6" t="s">
+        <v>494</v>
+      </c>
+      <c r="BP6" t="s">
+        <v>501</v>
+      </c>
+      <c r="BQ6" t="s">
+        <v>509</v>
+      </c>
+      <c r="BR6" t="s">
+        <v>517</v>
+      </c>
+      <c r="BS6" t="s">
+        <v>524</v>
+      </c>
+      <c r="BT6" t="s">
+        <v>532</v>
+      </c>
+      <c r="BU6" t="s">
+        <v>539</v>
+      </c>
+      <c r="BV6" t="s">
+        <v>547</v>
+      </c>
+      <c r="BW6" t="s">
+        <v>555</v>
+      </c>
+      <c r="BX6" t="s">
+        <v>563</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>569</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>577</v>
+      </c>
+      <c r="CB6" t="s">
+        <v>591</v>
+      </c>
+      <c r="CC6" t="s">
+        <v>598</v>
+      </c>
+      <c r="CD6" t="s">
+        <v>605</v>
+      </c>
+      <c r="CE6" t="s">
+        <v>612</v>
+      </c>
+      <c r="CF6" t="s">
+        <v>619</v>
+      </c>
+      <c r="CG6" t="s">
+        <v>626</v>
+      </c>
+      <c r="CH6" t="s">
+        <v>633</v>
+      </c>
+      <c r="CJ6" t="s">
+        <v>645</v>
+      </c>
+      <c r="CK6" t="s">
+        <v>653</v>
+      </c>
+      <c r="CL6" t="s">
+        <v>660</v>
+      </c>
+      <c r="CM6" t="s">
+        <v>667</v>
+      </c>
+      <c r="CN6" t="s">
+        <v>674</v>
+      </c>
+      <c r="CO6" t="s">
+        <v>682</v>
+      </c>
+      <c r="CP6" t="s">
+        <v>689</v>
+      </c>
+      <c r="CQ6" t="s">
+        <v>697</v>
+      </c>
+      <c r="CR6" t="s">
+        <v>705</v>
+      </c>
+      <c r="CS6" t="s">
+        <v>713</v>
+      </c>
+      <c r="CT6" t="s">
+        <v>721</v>
+      </c>
+      <c r="CU6" t="s">
+        <v>728</v>
+      </c>
+      <c r="CV6" t="s">
+        <v>734</v>
+      </c>
+      <c r="CW6" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="7" spans="1:101">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" t="s">
+        <v>100</v>
+      </c>
+      <c r="N7" t="s">
+        <v>106</v>
+      </c>
+      <c r="O7" t="s">
+        <v>115</v>
+      </c>
+      <c r="P7" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>131</v>
+      </c>
+      <c r="R7" t="s">
+        <v>138</v>
+      </c>
+      <c r="S7" t="s">
+        <v>145</v>
+      </c>
+      <c r="T7" t="s">
+        <v>152</v>
+      </c>
+      <c r="V7" t="s">
+        <v>166</v>
+      </c>
+      <c r="W7" t="s">
+        <v>174</v>
+      </c>
+      <c r="X7" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>227</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>242</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>257</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>272</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>279</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>286</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>249</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>306</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>313</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>321</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>328</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>335</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>343</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>351</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>359</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>366</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>373</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>380</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>394</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>401</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>409</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>416</v>
+      </c>
+      <c r="BE7" t="s">
+        <v>423</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>430</v>
+      </c>
+      <c r="BG7" t="s">
+        <v>438</v>
+      </c>
+      <c r="BH7" t="s">
+        <v>446</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>454</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>182</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>473</v>
+      </c>
+      <c r="BM7" t="s">
+        <v>481</v>
+      </c>
+      <c r="BN7" t="s">
+        <v>489</v>
+      </c>
+      <c r="BO7" t="s">
+        <v>495</v>
+      </c>
+      <c r="BP7" t="s">
+        <v>502</v>
+      </c>
+      <c r="BQ7" t="s">
+        <v>510</v>
+      </c>
+      <c r="BR7" t="s">
+        <v>518</v>
+      </c>
+      <c r="BS7" t="s">
+        <v>525</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>533</v>
+      </c>
+      <c r="BU7" t="s">
+        <v>540</v>
+      </c>
+      <c r="BV7" t="s">
+        <v>548</v>
+      </c>
+      <c r="BW7" t="s">
+        <v>556</v>
+      </c>
+      <c r="BX7" t="s">
+        <v>564</v>
+      </c>
+      <c r="BY7" t="s">
+        <v>570</v>
+      </c>
+      <c r="BZ7" t="s">
+        <v>578</v>
+      </c>
+      <c r="CA7" t="s">
+        <v>473</v>
+      </c>
+      <c r="CB7" t="s">
+        <v>592</v>
+      </c>
+      <c r="CC7" t="s">
+        <v>328</v>
+      </c>
+      <c r="CD7" t="s">
+        <v>606</v>
+      </c>
+      <c r="CE7" t="s">
+        <v>613</v>
+      </c>
+      <c r="CG7" t="s">
+        <v>30</v>
+      </c>
+      <c r="CI7" t="s">
+        <v>639</v>
+      </c>
+      <c r="CJ7" t="s">
+        <v>646</v>
+      </c>
+      <c r="CK7" t="s">
+        <v>654</v>
+      </c>
+      <c r="CM7" t="s">
+        <v>548</v>
+      </c>
+      <c r="CN7" t="s">
+        <v>675</v>
+      </c>
+      <c r="CO7" t="s">
+        <v>683</v>
+      </c>
+      <c r="CP7" t="s">
+        <v>690</v>
+      </c>
+      <c r="CQ7" t="s">
+        <v>698</v>
+      </c>
+      <c r="CR7" t="s">
+        <v>706</v>
+      </c>
+      <c r="CS7" t="s">
+        <v>714</v>
+      </c>
+      <c r="CT7" t="s">
+        <v>722</v>
+      </c>
+      <c r="CV7" t="s">
+        <v>735</v>
+      </c>
+      <c r="CW7" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="8" spans="1:101">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" t="s">
+        <v>87</v>
+      </c>
+      <c r="L8" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" t="s">
+        <v>101</v>
+      </c>
+      <c r="N8" t="s">
+        <v>107</v>
+      </c>
+      <c r="O8" t="s">
+        <v>116</v>
+      </c>
+      <c r="P8" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>132</v>
+      </c>
+      <c r="R8" t="s">
+        <v>139</v>
+      </c>
+      <c r="S8" t="s">
+        <v>146</v>
+      </c>
+      <c r="T8" t="s">
+        <v>153</v>
+      </c>
+      <c r="U8" t="s">
+        <v>159</v>
+      </c>
+      <c r="V8" t="s">
+        <v>167</v>
+      </c>
+      <c r="W8" t="s">
+        <v>175</v>
+      </c>
+      <c r="X8" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>198</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>206</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>212</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>235</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>243</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>258</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>265</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>273</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>287</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>294</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>307</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>314</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>322</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>329</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>336</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>344</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>352</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>360</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>367</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>374</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>381</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>387</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>395</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>402</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>410</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>417</v>
+      </c>
+      <c r="BE8" t="s">
+        <v>424</v>
+      </c>
+      <c r="BF8" t="s">
+        <v>431</v>
+      </c>
+      <c r="BG8" t="s">
+        <v>439</v>
+      </c>
+      <c r="BH8" t="s">
+        <v>447</v>
+      </c>
+      <c r="BI8" t="s">
+        <v>455</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>461</v>
+      </c>
+      <c r="BK8" t="s">
+        <v>467</v>
+      </c>
+      <c r="BL8" t="s">
+        <v>474</v>
+      </c>
+      <c r="BM8" t="s">
+        <v>482</v>
+      </c>
+      <c r="BN8" t="s">
+        <v>490</v>
+      </c>
+      <c r="BO8" t="s">
+        <v>496</v>
+      </c>
+      <c r="BP8" t="s">
+        <v>503</v>
+      </c>
+      <c r="BQ8" t="s">
+        <v>511</v>
+      </c>
+      <c r="BR8" t="s">
+        <v>519</v>
+      </c>
+      <c r="BS8" t="s">
+        <v>526</v>
+      </c>
+      <c r="BT8" t="s">
+        <v>534</v>
+      </c>
+      <c r="BU8" t="s">
+        <v>541</v>
+      </c>
+      <c r="BV8" t="s">
+        <v>549</v>
+      </c>
+      <c r="BW8" t="s">
+        <v>557</v>
+      </c>
+      <c r="BX8" t="s">
+        <v>565</v>
+      </c>
+      <c r="BY8" t="s">
+        <v>571</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>579</v>
+      </c>
+      <c r="CA8" t="s">
+        <v>585</v>
+      </c>
+      <c r="CB8" t="s">
+        <v>593</v>
+      </c>
+      <c r="CC8" t="s">
+        <v>599</v>
+      </c>
+      <c r="CD8" t="s">
+        <v>607</v>
+      </c>
+      <c r="CE8" t="s">
+        <v>614</v>
+      </c>
+      <c r="CF8" t="s">
+        <v>620</v>
+      </c>
+      <c r="CG8" t="s">
+        <v>627</v>
+      </c>
+      <c r="CH8" t="s">
+        <v>634</v>
+      </c>
+      <c r="CI8" t="s">
+        <v>640</v>
+      </c>
+      <c r="CJ8" t="s">
+        <v>647</v>
+      </c>
+      <c r="CK8" t="s">
+        <v>655</v>
+      </c>
+      <c r="CL8" t="s">
+        <v>661</v>
+      </c>
+      <c r="CM8" t="s">
+        <v>668</v>
+      </c>
+      <c r="CN8" t="s">
+        <v>676</v>
+      </c>
+      <c r="CO8" t="s">
+        <v>684</v>
+      </c>
+      <c r="CP8" t="s">
+        <v>691</v>
+      </c>
+      <c r="CQ8" t="s">
+        <v>699</v>
+      </c>
+      <c r="CR8" t="s">
+        <v>707</v>
+      </c>
+      <c r="CS8" t="s">
+        <v>715</v>
+      </c>
+      <c r="CT8" t="s">
+        <v>723</v>
+      </c>
+      <c r="CU8" t="s">
+        <v>729</v>
+      </c>
+      <c r="CV8" t="s">
+        <v>736</v>
+      </c>
+      <c r="CW8" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="9" spans="1:101">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AP9" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="AQ9" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="AR9" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="AS9" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AT9" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="BA9" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="BB9" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="BC9" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="BD9" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="BE9" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="BF9" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="BG9" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="BH9" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="BI9" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="BJ9" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="BK9" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="BL9" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="BM9" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="BN9" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="BO9" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="BP9" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="BQ9" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="BR9" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="BS9" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="BT9" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="BU9" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="BV9" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="BW9" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="BX9" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="BY9" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="BZ9" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="CA9" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="CB9" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="CC9" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="CD9" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="CE9" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="CF9" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="CG9" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="CH9" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="CI9" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="CJ9" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="CK9" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="CL9" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="CM9" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="CN9" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="CO9" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="CP9" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="CQ9" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="CR9" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="CS9" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="CT9" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="CU9" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="CV9" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="CW9" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="10" spans="1:98">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="AS10" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AT10" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="BB10" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="BF10" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="BG10" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="BH10" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="BL10" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="BM10" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="BP10" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="BQ10" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="BR10" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="BS10" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="BU10" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="BV10" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="BW10" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BY10" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="BZ10" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="CA10" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="CC10" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="CF10" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="CG10" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="CJ10" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="CL10" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="CM10" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="CN10" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="CP10" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="CQ10" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="CR10" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="CS10" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="CT10" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="11" spans="1:98">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>9</v>
+      </c>
+      <c r="P11">
+        <v>6</v>
+      </c>
+      <c r="U11">
+        <v>6</v>
+      </c>
+      <c r="V11">
+        <v>6</v>
+      </c>
+      <c r="W11">
+        <v>4</v>
+      </c>
+      <c r="X11">
+        <v>4</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>2</v>
+      </c>
+      <c r="AC11">
+        <v>3</v>
+      </c>
+      <c r="AD11">
+        <v>8</v>
+      </c>
+      <c r="AE11">
+        <v>7</v>
+      </c>
+      <c r="AG11">
+        <v>3</v>
+      </c>
+      <c r="AI11">
+        <v>6</v>
+      </c>
+      <c r="AJ11">
+        <v>4</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>3</v>
+      </c>
+      <c r="AS11">
+        <v>9</v>
+      </c>
+      <c r="AT11">
+        <v>5</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AZ11">
+        <v>10</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
+      <c r="BF11">
+        <v>1</v>
+      </c>
+      <c r="BG11">
+        <v>6</v>
+      </c>
+      <c r="BH11">
+        <v>3</v>
+      </c>
+      <c r="BL11">
+        <v>10</v>
+      </c>
+      <c r="BM11">
+        <v>3</v>
+      </c>
+      <c r="BP11">
+        <v>3</v>
+      </c>
+      <c r="BQ11">
+        <v>4</v>
+      </c>
+      <c r="BR11">
+        <v>0</v>
+      </c>
+      <c r="BS11">
+        <v>2</v>
+      </c>
+      <c r="BU11">
+        <v>5</v>
+      </c>
+      <c r="BV11">
+        <v>4</v>
+      </c>
+      <c r="BW11">
+        <v>9</v>
+      </c>
+      <c r="BY11">
+        <v>4</v>
+      </c>
+      <c r="BZ11">
+        <v>10</v>
+      </c>
+      <c r="CA11">
+        <v>3</v>
+      </c>
+      <c r="CC11">
+        <v>1</v>
+      </c>
+      <c r="CF11">
+        <v>1</v>
+      </c>
+      <c r="CG11">
+        <v>4</v>
+      </c>
+      <c r="CJ11">
+        <v>2</v>
+      </c>
+      <c r="CL11">
+        <v>7</v>
+      </c>
+      <c r="CM11">
+        <v>3</v>
+      </c>
+      <c r="CN11">
+        <v>1</v>
+      </c>
+      <c r="CP11">
+        <v>2</v>
+      </c>
+      <c r="CQ11">
+        <v>3</v>
+      </c>
+      <c r="CR11">
+        <v>6</v>
+      </c>
+      <c r="CS11">
+        <v>8</v>
+      </c>
+      <c r="CT11">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" ht="14.25" spans="1:11">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6476,7 +9522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" ht="14.25" spans="1:9">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6502,7 +9548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" ht="14.25" spans="1:9">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6531,7 +9577,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" ht="14.25" spans="1:11">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6566,7 +9612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:11">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>